<commit_message>
[ADD] 필요한 file 생성
</commit_message>
<xml_diff>
--- a/algorithm/WBS.xlsx
+++ b/algorithm/WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365inha-my.sharepoint.com/personal/22191082_office_inha_ac_kr/Documents/Machine Learning/Project/trading-system/algorithm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1787" documentId="13_ncr:1_{F524BCF4-B8E0-4A99-AD4E-A3303B5946CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECDF54D3-AD02-444D-B4B8-4ED57558B5B9}"/>
+  <xr:revisionPtr revIDLastSave="1939" documentId="13_ncr:1_{F524BCF4-B8E0-4A99-AD4E-A3303B5946CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0380ED29-4001-4D0A-A52D-EB5EF6E1C3E4}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{18AD7D50-32B8-4333-8B2F-86B153CFEE95}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="일정" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">일정!$A$1:$E$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">일정!$A$1:$E$46</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>우선순위</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -59,22 +59,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Interface 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DBHandler 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Engine, CollectionEngine, InvestmentEngine 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model, CollectionModel, InvestmentModel 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Database 구축</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -111,38 +95,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CollectionModel 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollectionModel_Y 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollectionModel_J 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CollectionModel_L 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvestmentModel 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvestmentModel_Y 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvestmentModel_J 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvestmentModel_L 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Monitoring system 구축</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -179,14 +131,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1.1.1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  계좌 개설</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>서버 할당</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -200,6 +144,46 @@
   </si>
   <si>
     <t>Stop - DataCollection, Invest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하위 공통 module(common) 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collector 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Investor 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine(abstract class) 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계좌 개설</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine(subclass).collect_data() 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>collect_data() 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine(subclass).get_action() 개발</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_action() 개발</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -740,40 +724,40 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,7 +790,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>100630</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>5604</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -823,7 +807,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="6448775" y="423213"/>
-          <a:ext cx="147905" cy="7545291"/>
+          <a:ext cx="147905" cy="9012141"/>
           <a:chOff x="5866942" y="-412079"/>
           <a:chExt cx="249471" cy="6465878"/>
         </a:xfrm>
@@ -1293,10 +1277,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R1048550"/>
+  <dimension ref="A1:R1048557"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1310,65 +1294,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="40" t="s">
+      <c r="A1" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="44"/>
+      <c r="F1" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="45"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="50"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -1391,13 +1375,13 @@
         <v>0.1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="13">
         <v>0</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="36"/>
@@ -1418,13 +1402,13 @@
         <v>0.2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="13">
         <v>0</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="36"/>
@@ -1445,13 +1429,13 @@
         <v>0.3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13">
         <v>0</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="36"/>
@@ -1472,13 +1456,13 @@
         <v>0.4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="13">
         <v>0</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="36"/>
@@ -1499,7 +1483,7 @@
         <v>0.5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C8" s="13">
         <v>0</v>
@@ -1566,13 +1550,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C11" s="13">
         <v>0</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="36"/>
@@ -1589,20 +1573,22 @@
       <c r="Q11" s="18"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>35</v>
+      <c r="A12" s="17">
+        <v>1.2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C12" s="13">
-        <v>4</v>
-      </c>
-      <c r="D12" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="37"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="3"/>
       <c r="J12" s="1"/>
       <c r="K12" s="2"/>
@@ -1615,16 +1601,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C13" s="13">
         <v>0</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="36"/>
@@ -1642,16 +1628,16 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C14" s="13">
         <v>0</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="36"/>
@@ -1669,16 +1655,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C15" s="13">
         <v>0</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="36"/>
@@ -1718,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -1741,13 +1727,13 @@
         <v>2.1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="13">
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="36"/>
@@ -1768,13 +1754,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" s="13">
         <v>1</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="36"/>
@@ -1814,7 +1800,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -1832,49 +1818,41 @@
       <c r="P21" s="32"/>
       <c r="Q21" s="34"/>
     </row>
-    <row r="22" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="17">
         <v>3.1</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>19</v>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="20"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
-        <v>3.2</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="13">
-        <v>2</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="A23" s="19"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
       <c r="J23" s="10"/>
@@ -1886,114 +1864,110 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="20"/>
     </row>
-    <row r="24" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
-        <v>3.3</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="13">
-        <v>2</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="20"/>
-    </row>
-    <row r="25" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+    <row r="24" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="34"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="E25" s="13"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="8"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="20"/>
-    </row>
-    <row r="26" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="29">
-        <v>4</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="34"/>
-    </row>
-    <row r="27" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="13">
-        <v>3</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="20"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="18"/>
+    </row>
+    <row r="27" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="34"/>
     </row>
     <row r="28" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C28" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="36"/>
@@ -2002,8 +1976,8 @@
       <c r="I28" s="9"/>
       <c r="J28" s="10"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="3"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="10"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
@@ -2011,16 +1985,16 @@
     </row>
     <row r="29" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
-        <v>4.3</v>
+        <v>5.2</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C29" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="36"/>
@@ -2037,92 +2011,92 @@
       <c r="Q29" s="20"/>
     </row>
     <row r="30" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="A30" s="19">
+        <v>5.3</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="13">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="E30" s="13"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="9"/>
       <c r="J30" s="10"/>
       <c r="K30" s="8"/>
       <c r="L30" s="2"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="18"/>
-    </row>
-    <row r="31" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29">
-        <v>5</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="34"/>
-    </row>
-    <row r="32" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="15">
-        <v>5</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="20"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="20"/>
+    </row>
+    <row r="31" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="18"/>
+    </row>
+    <row r="32" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29">
+        <v>6</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="34"/>
     </row>
     <row r="33" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
-        <v>5.2</v>
+        <v>6.1</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="15">
-        <v>5</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="C33" s="13">
+        <v>1</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
       <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="10"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -2134,175 +2108,354 @@
     </row>
     <row r="34" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="15">
-        <v>5</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="C34" s="13">
+        <v>1</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
       <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="10"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="9"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="3"/>
       <c r="N34" s="10"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="20"/>
     </row>
     <row r="35" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="A35" s="19">
+        <v>6.3</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="13">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="9"/>
       <c r="J35" s="10"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="9"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="3"/>
       <c r="N35" s="10"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="20"/>
     </row>
-    <row r="36" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29">
-        <v>6</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="30">
-        <v>6</v>
-      </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="34"/>
+    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="19">
+        <v>6.4</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="13">
+        <v>2</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="20"/>
     </row>
     <row r="37" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="10"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="9"/>
       <c r="J37" s="10"/>
       <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="9"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="3"/>
       <c r="N37" s="10"/>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="20"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="18"/>
-    </row>
-    <row r="39" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="23">
-        <f>SUM(F39:Q39)</f>
+    <row r="38" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="29">
+        <v>7</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="34"/>
+    </row>
+    <row r="39" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>7.1</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="15">
+        <v>3</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="20"/>
+    </row>
+    <row r="40" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="19">
+        <v>7.2</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="15">
+        <v>3</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="20"/>
+    </row>
+    <row r="41" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19">
+        <v>7.3</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="15">
+        <v>3</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="20"/>
+    </row>
+    <row r="42" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="20"/>
+    </row>
+    <row r="43" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="29">
+        <v>8</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="34"/>
+    </row>
+    <row r="44" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>8.1</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="15">
+        <v>4</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="20"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="18"/>
+    </row>
+    <row r="46" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="23">
+        <f>SUM(F46:Q46)</f>
         <v>0</v>
       </c>
-      <c r="F39" s="25">
-        <f>SUM(F3:F38)</f>
+      <c r="F46" s="25">
+        <f>SUM(F3:F45)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="25">
-        <f>SUM(G3:G38)</f>
+      <c r="G46" s="25">
+        <f>SUM(G3:G45)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="25">
-        <f t="shared" ref="H39:Q39" si="0">SUM(H3:H38)</f>
+      <c r="H46" s="25">
+        <f t="shared" ref="H46:Q46" si="0">SUM(H3:H45)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="26">
+      <c r="I46" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="27">
+      <c r="J46" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="25">
+      <c r="K46" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L39" s="25">
+      <c r="L46" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M39" s="26">
+      <c r="M46" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N39" s="27">
+      <c r="N46" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O39" s="25">
+      <c r="O46" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P39" s="25">
+      <c r="P46" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q39" s="28">
+      <c r="Q46" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R39" s="16"/>
-    </row>
-    <row r="1048550" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="R46" s="16"/>
+    </row>
+    <row r="1048557" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="F1:I2"/>
@@ -2322,15 +2475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AEEA0C3368F6CA4FAFB457DB6053378D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2e02f33cedf3fabcb08e79664a68bc6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad079af5-13e3-437d-9c94-eab00b349c45" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f85069d2f559aa63ffacec4c071c7db1" ns2:_="">
     <xsd:import namespace="ad079af5-13e3-437d-9c94-eab00b349c45"/>
@@ -2514,6 +2658,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2521,14 +2674,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC61BBFB-7E63-4FB0-837B-5B35DE1045FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C27BD4-BE0E-4C00-86D5-55262742EC2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2546,6 +2691,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC61BBFB-7E63-4FB0-837B-5B35DE1045FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{605504CE-7E87-40CB-B0FC-2E19CA59A81F}">
   <ds:schemaRefs>

</xml_diff>